<commit_message>
modif pour ajout des exos et compilation double avec pythontex et pdflatex
</commit_message>
<xml_diff>
--- a/inventaire_exos.xlsx
+++ b/inventaire_exos.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="13" uniqueCount="13">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="16" uniqueCount="15">
   <si>
     <t>Domaine</t>
   </si>
@@ -66,6 +66,12 @@
   </si>
   <si>
     <t>Types simples</t>
+  </si>
+  <si>
+    <t>PYB-100</t>
+  </si>
+  <si>
+    <t>Types composés</t>
   </si>
 </sst>
 </file>
@@ -380,10 +386,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F4"/>
+  <dimension ref="A1:F5"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="C4" sqref="C4"/>
+      <selection activeCell="C5" sqref="C5"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -440,6 +446,17 @@
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A4" t="s">
+        <v>10</v>
+      </c>
+      <c r="B4" t="s">
+        <v>13</v>
+      </c>
+      <c r="C4" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="5" spans="1:6" x14ac:dyDescent="0.2">
+      <c r="A5" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
maj cours 4 et TP03
</commit_message>
<xml_diff>
--- a/inventaire_exos.xlsx
+++ b/inventaire_exos.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="200" yWindow="460" windowWidth="24560" windowHeight="13440" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14560" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="exos" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="133" uniqueCount="61">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="75">
   <si>
     <t>Domaine</t>
   </si>
@@ -210,6 +210,48 @@
   </si>
   <si>
     <t>Boucles "while"</t>
+  </si>
+  <si>
+    <t>plot</t>
+  </si>
+  <si>
+    <t>PLT-002</t>
+  </si>
+  <si>
+    <t>Tracé de courbes</t>
+  </si>
+  <si>
+    <t>PLT-003</t>
+  </si>
+  <si>
+    <t>Exemple avancé</t>
+  </si>
+  <si>
+    <t>PYB-308</t>
+  </si>
+  <si>
+    <t>Fonctions en Python</t>
+  </si>
+  <si>
+    <t>301+305</t>
+  </si>
+  <si>
+    <t>400,401,404</t>
+  </si>
+  <si>
+    <t>PYB-411</t>
+  </si>
+  <si>
+    <t>Boucles IF, FOR, WHILE</t>
+  </si>
+  <si>
+    <t>Algorithme glouton -- Problème du rendu de monnaie</t>
+  </si>
+  <si>
+    <t>ALGO-012</t>
+  </si>
+  <si>
+    <t>algo</t>
   </si>
 </sst>
 </file>
@@ -524,10 +566,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F42"/>
+  <dimension ref="A1:F47"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A14" workbookViewId="0">
-      <selection activeCell="C42" sqref="C42"/>
+    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
+      <selection activeCell="A47" sqref="A47"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -919,7 +961,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="33" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="33" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A33" t="s">
         <v>10</v>
       </c>
@@ -930,7 +972,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="34" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="34" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A34" t="s">
         <v>10</v>
       </c>
@@ -941,7 +983,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="35" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="35" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A35" t="s">
         <v>10</v>
       </c>
@@ -952,7 +994,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="36" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>10</v>
       </c>
@@ -963,7 +1005,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="37" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="37" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A37" t="s">
         <v>10</v>
       </c>
@@ -974,7 +1016,7 @@
         <v>37</v>
       </c>
     </row>
-    <row r="38" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="38" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A38" t="s">
         <v>10</v>
       </c>
@@ -985,41 +1027,102 @@
         <v>37</v>
       </c>
     </row>
-    <row r="39" spans="1:3" x14ac:dyDescent="0.2">
+    <row r="39" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A39" t="s">
         <v>10</v>
       </c>
       <c r="B39" t="s">
+        <v>66</v>
+      </c>
+      <c r="C39" t="s">
+        <v>67</v>
+      </c>
+      <c r="E39" t="s">
+        <v>68</v>
+      </c>
+    </row>
+    <row r="40" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A40" t="s">
+        <v>10</v>
+      </c>
+      <c r="B40" t="s">
         <v>55</v>
       </c>
-      <c r="C39" t="s">
+      <c r="C40" t="s">
         <v>56</v>
       </c>
     </row>
-    <row r="40" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A40" t="s">
-        <v>10</v>
-      </c>
-      <c r="B40" t="s">
+    <row r="41" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A41" t="s">
+        <v>10</v>
+      </c>
+      <c r="B41" t="s">
         <v>57</v>
       </c>
-      <c r="C40" t="s">
+      <c r="C41" t="s">
         <v>59</v>
       </c>
     </row>
-    <row r="41" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A41" t="s">
-        <v>10</v>
-      </c>
-      <c r="B41" t="s">
+    <row r="42" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A42" t="s">
+        <v>10</v>
+      </c>
+      <c r="B42" t="s">
         <v>58</v>
       </c>
-      <c r="C41" t="s">
+      <c r="C42" t="s">
         <v>60</v>
       </c>
     </row>
-    <row r="42" spans="1:3" x14ac:dyDescent="0.2">
-      <c r="A42" t="s">
+    <row r="43" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A43" t="s">
+        <v>10</v>
+      </c>
+      <c r="B43" t="s">
+        <v>70</v>
+      </c>
+      <c r="C43" t="s">
+        <v>71</v>
+      </c>
+      <c r="E43" t="s">
+        <v>69</v>
+      </c>
+    </row>
+    <row r="44" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A44" t="s">
+        <v>61</v>
+      </c>
+      <c r="B44" t="s">
+        <v>62</v>
+      </c>
+      <c r="C44" t="s">
+        <v>63</v>
+      </c>
+    </row>
+    <row r="45" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A45" t="s">
+        <v>61</v>
+      </c>
+      <c r="B45" t="s">
+        <v>64</v>
+      </c>
+      <c r="C45" t="s">
+        <v>65</v>
+      </c>
+    </row>
+    <row r="46" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A46" t="s">
+        <v>74</v>
+      </c>
+      <c r="B46" t="s">
+        <v>73</v>
+      </c>
+      <c r="C46" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="47" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A47" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
modification TP03 avec corrigé
</commit_message>
<xml_diff>
--- a/inventaire_exos.xlsx
+++ b/inventaire_exos.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="25600" windowHeight="14560" tabRatio="500"/>
+    <workbookView xWindow="0" yWindow="660" windowWidth="25600" windowHeight="14520" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="exos" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="150" uniqueCount="75">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="153" uniqueCount="76">
   <si>
     <t>Domaine</t>
   </si>
@@ -248,10 +248,13 @@
     <t>Algorithme glouton -- Problème du rendu de monnaie</t>
   </si>
   <si>
-    <t>ALGO-012</t>
-  </si>
-  <si>
     <t>algo</t>
+  </si>
+  <si>
+    <t>consignes_TP3</t>
+  </si>
+  <si>
+    <t>ALG-012</t>
   </si>
 </sst>
 </file>
@@ -566,17 +569,17 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F47"/>
+  <dimension ref="A1:F48"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A19" workbookViewId="0">
-      <selection activeCell="A47" sqref="A47"/>
+    <sheetView tabSelected="1" topLeftCell="A28" workbookViewId="0">
+      <selection activeCell="B48" sqref="B48"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
   <cols>
     <col min="1" max="1" width="12.5" bestFit="1" customWidth="1"/>
     <col min="2" max="2" width="13.1640625" bestFit="1" customWidth="1"/>
-    <col min="3" max="3" width="42" bestFit="1" customWidth="1"/>
+    <col min="3" max="3" width="74.5" bestFit="1" customWidth="1"/>
     <col min="4" max="4" width="17.1640625" customWidth="1"/>
     <col min="5" max="5" width="13" bestFit="1" customWidth="1"/>
     <col min="6" max="6" width="17.83203125" bestFit="1" customWidth="1"/>
@@ -615,13 +618,13 @@
     </row>
     <row r="3" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A3" t="s">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="B3" t="s">
-        <v>6</v>
+        <v>74</v>
       </c>
       <c r="C3" t="s">
-        <v>9</v>
+        <v>51</v>
       </c>
     </row>
     <row r="4" spans="1:6" x14ac:dyDescent="0.2">
@@ -629,10 +632,10 @@
         <v>5</v>
       </c>
       <c r="B4" t="s">
-        <v>47</v>
+        <v>6</v>
       </c>
       <c r="C4" t="s">
-        <v>49</v>
+        <v>9</v>
       </c>
     </row>
     <row r="5" spans="1:6" x14ac:dyDescent="0.2">
@@ -640,24 +643,21 @@
         <v>5</v>
       </c>
       <c r="B5" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C5" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B6" t="s">
-        <v>11</v>
+        <v>48</v>
       </c>
       <c r="C6" t="s">
-        <v>12</v>
-      </c>
-      <c r="E6" t="s">
-        <v>46</v>
+        <v>52</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -665,10 +665,10 @@
         <v>10</v>
       </c>
       <c r="B7" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="C7" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E7" t="s">
         <v>46</v>
@@ -679,7 +679,7 @@
         <v>10</v>
       </c>
       <c r="B8" t="s">
-        <v>53</v>
+        <v>25</v>
       </c>
       <c r="C8" t="s">
         <v>14</v>
@@ -693,18 +693,21 @@
         <v>10</v>
       </c>
       <c r="B9" t="s">
-        <v>13</v>
+        <v>53</v>
       </c>
       <c r="C9" t="s">
         <v>14</v>
       </c>
+      <c r="E9" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
         <v>10</v>
       </c>
       <c r="B10" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C10" t="s">
         <v>14</v>
@@ -715,7 +718,7 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C11" t="s">
         <v>14</v>
@@ -726,7 +729,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C12" t="s">
         <v>14</v>
@@ -737,7 +740,7 @@
         <v>10</v>
       </c>
       <c r="B13" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C13" t="s">
         <v>14</v>
@@ -748,7 +751,7 @@
         <v>10</v>
       </c>
       <c r="B14" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C14" t="s">
         <v>14</v>
@@ -759,7 +762,7 @@
         <v>10</v>
       </c>
       <c r="B15" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C15" t="s">
         <v>14</v>
@@ -770,7 +773,7 @@
         <v>10</v>
       </c>
       <c r="B16" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C16" t="s">
         <v>14</v>
@@ -781,7 +784,7 @@
         <v>10</v>
       </c>
       <c r="B17" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C17" t="s">
         <v>14</v>
@@ -792,13 +795,10 @@
         <v>10</v>
       </c>
       <c r="B18" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C18" t="s">
-        <v>23</v>
-      </c>
-      <c r="E18" t="s">
-        <v>46</v>
+        <v>14</v>
       </c>
     </row>
     <row r="19" spans="1:5" x14ac:dyDescent="0.2">
@@ -806,7 +806,7 @@
         <v>10</v>
       </c>
       <c r="B19" t="s">
-        <v>54</v>
+        <v>24</v>
       </c>
       <c r="C19" t="s">
         <v>23</v>
@@ -820,18 +820,21 @@
         <v>10</v>
       </c>
       <c r="B20" t="s">
-        <v>26</v>
+        <v>54</v>
       </c>
       <c r="C20" t="s">
         <v>23</v>
       </c>
+      <c r="E20" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="21" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A21" t="s">
         <v>10</v>
       </c>
       <c r="B21" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C21" t="s">
         <v>23</v>
@@ -842,7 +845,7 @@
         <v>10</v>
       </c>
       <c r="B22" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C22" t="s">
         <v>23</v>
@@ -853,7 +856,7 @@
         <v>10</v>
       </c>
       <c r="B23" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C23" t="s">
         <v>23</v>
@@ -864,7 +867,7 @@
         <v>10</v>
       </c>
       <c r="B24" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C24" t="s">
         <v>23</v>
@@ -875,7 +878,7 @@
         <v>10</v>
       </c>
       <c r="B25" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C25" t="s">
         <v>23</v>
@@ -886,7 +889,7 @@
         <v>10</v>
       </c>
       <c r="B26" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C26" t="s">
         <v>23</v>
@@ -897,7 +900,7 @@
         <v>10</v>
       </c>
       <c r="B27" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C27" t="s">
         <v>23</v>
@@ -908,7 +911,7 @@
         <v>10</v>
       </c>
       <c r="B28" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C28" t="s">
         <v>23</v>
@@ -919,7 +922,7 @@
         <v>10</v>
       </c>
       <c r="B29" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C29" t="s">
         <v>23</v>
@@ -930,13 +933,10 @@
         <v>10</v>
       </c>
       <c r="B30" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C30" t="s">
-        <v>37</v>
-      </c>
-      <c r="E30" t="s">
-        <v>46</v>
+        <v>23</v>
       </c>
     </row>
     <row r="31" spans="1:5" x14ac:dyDescent="0.2">
@@ -944,18 +944,21 @@
         <v>10</v>
       </c>
       <c r="B31" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C31" t="s">
         <v>37</v>
       </c>
+      <c r="E31" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="32" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A32" t="s">
         <v>10</v>
       </c>
       <c r="B32" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C32" t="s">
         <v>37</v>
@@ -966,7 +969,7 @@
         <v>10</v>
       </c>
       <c r="B33" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C33" t="s">
         <v>37</v>
@@ -977,7 +980,7 @@
         <v>10</v>
       </c>
       <c r="B34" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C34" t="s">
         <v>37</v>
@@ -988,7 +991,7 @@
         <v>10</v>
       </c>
       <c r="B35" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C35" t="s">
         <v>37</v>
@@ -999,7 +1002,7 @@
         <v>10</v>
       </c>
       <c r="B36" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C36" t="s">
         <v>37</v>
@@ -1010,7 +1013,7 @@
         <v>10</v>
       </c>
       <c r="B37" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C37" t="s">
         <v>37</v>
@@ -1021,7 +1024,7 @@
         <v>10</v>
       </c>
       <c r="B38" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C38" t="s">
         <v>37</v>
@@ -1032,13 +1035,10 @@
         <v>10</v>
       </c>
       <c r="B39" t="s">
-        <v>66</v>
+        <v>45</v>
       </c>
       <c r="C39" t="s">
-        <v>67</v>
-      </c>
-      <c r="E39" t="s">
-        <v>68</v>
+        <v>37</v>
       </c>
     </row>
     <row r="40" spans="1:5" x14ac:dyDescent="0.2">
@@ -1046,10 +1046,13 @@
         <v>10</v>
       </c>
       <c r="B40" t="s">
-        <v>55</v>
+        <v>66</v>
       </c>
       <c r="C40" t="s">
-        <v>56</v>
+        <v>67</v>
+      </c>
+      <c r="E40" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="41" spans="1:5" x14ac:dyDescent="0.2">
@@ -1057,10 +1060,10 @@
         <v>10</v>
       </c>
       <c r="B41" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C41" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="42" spans="1:5" x14ac:dyDescent="0.2">
@@ -1068,10 +1071,10 @@
         <v>10</v>
       </c>
       <c r="B42" t="s">
-        <v>58</v>
+        <v>57</v>
       </c>
       <c r="C42" t="s">
-        <v>60</v>
+        <v>59</v>
       </c>
     </row>
     <row r="43" spans="1:5" x14ac:dyDescent="0.2">
@@ -1079,24 +1082,24 @@
         <v>10</v>
       </c>
       <c r="B43" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="C43" t="s">
-        <v>71</v>
-      </c>
-      <c r="E43" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A44" t="s">
-        <v>61</v>
+        <v>10</v>
       </c>
       <c r="B44" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="C44" t="s">
-        <v>63</v>
+        <v>71</v>
+      </c>
+      <c r="E44" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
@@ -1104,25 +1107,36 @@
         <v>61</v>
       </c>
       <c r="B45" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C45" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A46" t="s">
-        <v>74</v>
+        <v>61</v>
       </c>
       <c r="B46" t="s">
-        <v>73</v>
+        <v>64</v>
       </c>
       <c r="C46" t="s">
-        <v>72</v>
+        <v>65</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A47" t="s">
+        <v>73</v>
+      </c>
+      <c r="B47" t="s">
+        <v>75</v>
+      </c>
+      <c r="C47" t="s">
+        <v>72</v>
+      </c>
+    </row>
+    <row r="48" spans="1:5" x14ac:dyDescent="0.2">
+      <c r="A48" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
modif cours 7 et TP06
</commit_message>
<xml_diff>
--- a/inventaire_exos.xlsx
+++ b/inventaire_exos.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="216" uniqueCount="116">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="234" uniqueCount="128">
   <si>
     <t>Domaine</t>
   </si>
@@ -375,6 +375,42 @@
   </si>
   <si>
     <t>TAB-026</t>
+  </si>
+  <si>
+    <t>fichiers</t>
+  </si>
+  <si>
+    <t>FIC-007</t>
+  </si>
+  <si>
+    <t>Classement de la "Saintélyon"</t>
+  </si>
+  <si>
+    <t>FIC-010</t>
+  </si>
+  <si>
+    <t>Traitement de données physiologiques</t>
+  </si>
+  <si>
+    <t>FIC-009</t>
+  </si>
+  <si>
+    <t>Analyse d'un dipôle électrique</t>
+  </si>
+  <si>
+    <t>FIC-011</t>
+  </si>
+  <si>
+    <t>Lecture d'un texte</t>
+  </si>
+  <si>
+    <t>consignes_TP6</t>
+  </si>
+  <si>
+    <t>FIC-012</t>
+  </si>
+  <si>
+    <t>Résultats de l'Embrunman</t>
   </si>
 </sst>
 </file>
@@ -689,10 +725,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F69"/>
+  <dimension ref="A1:F75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A44" workbookViewId="0">
-      <selection activeCell="B69" sqref="B69"/>
+    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
+      <selection activeCell="C74" sqref="C74"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -771,13 +807,13 @@
     </row>
     <row r="6" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A6" t="s">
-        <v>5</v>
+        <v>50</v>
       </c>
       <c r="B6" t="s">
-        <v>6</v>
+        <v>125</v>
       </c>
       <c r="C6" t="s">
-        <v>9</v>
+        <v>51</v>
       </c>
     </row>
     <row r="7" spans="1:6" x14ac:dyDescent="0.2">
@@ -785,10 +821,10 @@
         <v>5</v>
       </c>
       <c r="B7" t="s">
-        <v>47</v>
+        <v>6</v>
       </c>
       <c r="C7" t="s">
-        <v>49</v>
+        <v>9</v>
       </c>
     </row>
     <row r="8" spans="1:6" x14ac:dyDescent="0.2">
@@ -796,10 +832,10 @@
         <v>5</v>
       </c>
       <c r="B8" t="s">
-        <v>48</v>
+        <v>47</v>
       </c>
       <c r="C8" t="s">
-        <v>52</v>
+        <v>49</v>
       </c>
     </row>
     <row r="9" spans="1:6" x14ac:dyDescent="0.2">
@@ -807,24 +843,21 @@
         <v>5</v>
       </c>
       <c r="B9" t="s">
-        <v>97</v>
+        <v>48</v>
       </c>
       <c r="C9" t="s">
-        <v>96</v>
+        <v>52</v>
       </c>
     </row>
     <row r="10" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A10" t="s">
-        <v>10</v>
+        <v>5</v>
       </c>
       <c r="B10" t="s">
-        <v>11</v>
+        <v>97</v>
       </c>
       <c r="C10" t="s">
-        <v>12</v>
-      </c>
-      <c r="E10" t="s">
-        <v>46</v>
+        <v>96</v>
       </c>
     </row>
     <row r="11" spans="1:6" x14ac:dyDescent="0.2">
@@ -832,10 +865,10 @@
         <v>10</v>
       </c>
       <c r="B11" t="s">
-        <v>25</v>
+        <v>11</v>
       </c>
       <c r="C11" t="s">
-        <v>14</v>
+        <v>12</v>
       </c>
       <c r="E11" t="s">
         <v>46</v>
@@ -846,7 +879,7 @@
         <v>10</v>
       </c>
       <c r="B12" t="s">
-        <v>53</v>
+        <v>25</v>
       </c>
       <c r="C12" t="s">
         <v>14</v>
@@ -860,18 +893,21 @@
         <v>10</v>
       </c>
       <c r="B13" t="s">
-        <v>13</v>
+        <v>53</v>
       </c>
       <c r="C13" t="s">
         <v>14</v>
       </c>
+      <c r="E13" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="14" spans="1:6" x14ac:dyDescent="0.2">
       <c r="A14" t="s">
         <v>10</v>
       </c>
       <c r="B14" t="s">
-        <v>15</v>
+        <v>13</v>
       </c>
       <c r="C14" t="s">
         <v>14</v>
@@ -882,7 +918,7 @@
         <v>10</v>
       </c>
       <c r="B15" t="s">
-        <v>16</v>
+        <v>15</v>
       </c>
       <c r="C15" t="s">
         <v>14</v>
@@ -893,7 +929,7 @@
         <v>10</v>
       </c>
       <c r="B16" t="s">
-        <v>17</v>
+        <v>16</v>
       </c>
       <c r="C16" t="s">
         <v>14</v>
@@ -904,7 +940,7 @@
         <v>10</v>
       </c>
       <c r="B17" t="s">
-        <v>18</v>
+        <v>17</v>
       </c>
       <c r="C17" t="s">
         <v>14</v>
@@ -915,7 +951,7 @@
         <v>10</v>
       </c>
       <c r="B18" t="s">
-        <v>20</v>
+        <v>18</v>
       </c>
       <c r="C18" t="s">
         <v>14</v>
@@ -926,7 +962,7 @@
         <v>10</v>
       </c>
       <c r="B19" t="s">
-        <v>19</v>
+        <v>20</v>
       </c>
       <c r="C19" t="s">
         <v>14</v>
@@ -937,7 +973,7 @@
         <v>10</v>
       </c>
       <c r="B20" t="s">
-        <v>21</v>
+        <v>19</v>
       </c>
       <c r="C20" t="s">
         <v>14</v>
@@ -948,7 +984,7 @@
         <v>10</v>
       </c>
       <c r="B21" t="s">
-        <v>22</v>
+        <v>21</v>
       </c>
       <c r="C21" t="s">
         <v>14</v>
@@ -959,13 +995,10 @@
         <v>10</v>
       </c>
       <c r="B22" t="s">
-        <v>24</v>
+        <v>22</v>
       </c>
       <c r="C22" t="s">
-        <v>23</v>
-      </c>
-      <c r="E22" t="s">
-        <v>46</v>
+        <v>14</v>
       </c>
     </row>
     <row r="23" spans="1:5" x14ac:dyDescent="0.2">
@@ -973,7 +1006,7 @@
         <v>10</v>
       </c>
       <c r="B23" t="s">
-        <v>54</v>
+        <v>24</v>
       </c>
       <c r="C23" t="s">
         <v>23</v>
@@ -987,18 +1020,21 @@
         <v>10</v>
       </c>
       <c r="B24" t="s">
-        <v>26</v>
+        <v>54</v>
       </c>
       <c r="C24" t="s">
         <v>23</v>
       </c>
+      <c r="E24" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="25" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A25" t="s">
         <v>10</v>
       </c>
       <c r="B25" t="s">
-        <v>27</v>
+        <v>26</v>
       </c>
       <c r="C25" t="s">
         <v>23</v>
@@ -1009,7 +1045,7 @@
         <v>10</v>
       </c>
       <c r="B26" t="s">
-        <v>28</v>
+        <v>27</v>
       </c>
       <c r="C26" t="s">
         <v>23</v>
@@ -1020,7 +1056,7 @@
         <v>10</v>
       </c>
       <c r="B27" t="s">
-        <v>29</v>
+        <v>28</v>
       </c>
       <c r="C27" t="s">
         <v>23</v>
@@ -1031,7 +1067,7 @@
         <v>10</v>
       </c>
       <c r="B28" t="s">
-        <v>30</v>
+        <v>29</v>
       </c>
       <c r="C28" t="s">
         <v>23</v>
@@ -1042,7 +1078,7 @@
         <v>10</v>
       </c>
       <c r="B29" t="s">
-        <v>31</v>
+        <v>30</v>
       </c>
       <c r="C29" t="s">
         <v>23</v>
@@ -1053,7 +1089,7 @@
         <v>10</v>
       </c>
       <c r="B30" t="s">
-        <v>32</v>
+        <v>31</v>
       </c>
       <c r="C30" t="s">
         <v>23</v>
@@ -1064,7 +1100,7 @@
         <v>10</v>
       </c>
       <c r="B31" t="s">
-        <v>33</v>
+        <v>32</v>
       </c>
       <c r="C31" t="s">
         <v>23</v>
@@ -1075,7 +1111,7 @@
         <v>10</v>
       </c>
       <c r="B32" t="s">
-        <v>34</v>
+        <v>33</v>
       </c>
       <c r="C32" t="s">
         <v>23</v>
@@ -1086,7 +1122,7 @@
         <v>10</v>
       </c>
       <c r="B33" t="s">
-        <v>35</v>
+        <v>34</v>
       </c>
       <c r="C33" t="s">
         <v>23</v>
@@ -1097,13 +1133,10 @@
         <v>10</v>
       </c>
       <c r="B34" t="s">
-        <v>36</v>
+        <v>35</v>
       </c>
       <c r="C34" t="s">
-        <v>37</v>
-      </c>
-      <c r="E34" t="s">
-        <v>46</v>
+        <v>23</v>
       </c>
     </row>
     <row r="35" spans="1:5" x14ac:dyDescent="0.2">
@@ -1111,18 +1144,21 @@
         <v>10</v>
       </c>
       <c r="B35" t="s">
-        <v>38</v>
+        <v>36</v>
       </c>
       <c r="C35" t="s">
         <v>37</v>
       </c>
+      <c r="E35" t="s">
+        <v>46</v>
+      </c>
     </row>
     <row r="36" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A36" t="s">
         <v>10</v>
       </c>
       <c r="B36" t="s">
-        <v>39</v>
+        <v>38</v>
       </c>
       <c r="C36" t="s">
         <v>37</v>
@@ -1133,7 +1169,7 @@
         <v>10</v>
       </c>
       <c r="B37" t="s">
-        <v>40</v>
+        <v>39</v>
       </c>
       <c r="C37" t="s">
         <v>37</v>
@@ -1144,7 +1180,7 @@
         <v>10</v>
       </c>
       <c r="B38" t="s">
-        <v>41</v>
+        <v>40</v>
       </c>
       <c r="C38" t="s">
         <v>37</v>
@@ -1155,7 +1191,7 @@
         <v>10</v>
       </c>
       <c r="B39" t="s">
-        <v>42</v>
+        <v>41</v>
       </c>
       <c r="C39" t="s">
         <v>37</v>
@@ -1166,7 +1202,7 @@
         <v>10</v>
       </c>
       <c r="B40" t="s">
-        <v>43</v>
+        <v>42</v>
       </c>
       <c r="C40" t="s">
         <v>37</v>
@@ -1177,7 +1213,7 @@
         <v>10</v>
       </c>
       <c r="B41" t="s">
-        <v>44</v>
+        <v>43</v>
       </c>
       <c r="C41" t="s">
         <v>37</v>
@@ -1188,7 +1224,7 @@
         <v>10</v>
       </c>
       <c r="B42" t="s">
-        <v>45</v>
+        <v>44</v>
       </c>
       <c r="C42" t="s">
         <v>37</v>
@@ -1199,13 +1235,10 @@
         <v>10</v>
       </c>
       <c r="B43" t="s">
-        <v>66</v>
+        <v>45</v>
       </c>
       <c r="C43" t="s">
-        <v>67</v>
-      </c>
-      <c r="E43" t="s">
-        <v>68</v>
+        <v>37</v>
       </c>
     </row>
     <row r="44" spans="1:5" x14ac:dyDescent="0.2">
@@ -1213,10 +1246,13 @@
         <v>10</v>
       </c>
       <c r="B44" t="s">
-        <v>76</v>
+        <v>66</v>
       </c>
       <c r="C44" t="s">
-        <v>56</v>
+        <v>67</v>
+      </c>
+      <c r="E44" t="s">
+        <v>68</v>
       </c>
     </row>
     <row r="45" spans="1:5" x14ac:dyDescent="0.2">
@@ -1224,10 +1260,10 @@
         <v>10</v>
       </c>
       <c r="B45" t="s">
-        <v>77</v>
+        <v>76</v>
       </c>
       <c r="C45" t="s">
-        <v>78</v>
+        <v>56</v>
       </c>
     </row>
     <row r="46" spans="1:5" x14ac:dyDescent="0.2">
@@ -1235,10 +1271,10 @@
         <v>10</v>
       </c>
       <c r="B46" t="s">
-        <v>80</v>
+        <v>77</v>
       </c>
       <c r="C46" t="s">
-        <v>81</v>
+        <v>78</v>
       </c>
     </row>
     <row r="47" spans="1:5" x14ac:dyDescent="0.2">
@@ -1246,10 +1282,10 @@
         <v>10</v>
       </c>
       <c r="B47" t="s">
-        <v>84</v>
+        <v>80</v>
       </c>
       <c r="C47" t="s">
-        <v>85</v>
+        <v>81</v>
       </c>
     </row>
     <row r="48" spans="1:5" x14ac:dyDescent="0.2">
@@ -1257,10 +1293,10 @@
         <v>10</v>
       </c>
       <c r="B48" t="s">
-        <v>87</v>
+        <v>84</v>
       </c>
       <c r="C48" t="s">
-        <v>86</v>
+        <v>85</v>
       </c>
     </row>
     <row r="49" spans="1:5" x14ac:dyDescent="0.2">
@@ -1268,10 +1304,10 @@
         <v>10</v>
       </c>
       <c r="B49" t="s">
-        <v>55</v>
+        <v>87</v>
       </c>
       <c r="C49" t="s">
-        <v>56</v>
+        <v>86</v>
       </c>
     </row>
     <row r="50" spans="1:5" x14ac:dyDescent="0.2">
@@ -1279,10 +1315,10 @@
         <v>10</v>
       </c>
       <c r="B50" t="s">
-        <v>57</v>
+        <v>55</v>
       </c>
       <c r="C50" t="s">
-        <v>59</v>
+        <v>56</v>
       </c>
     </row>
     <row r="51" spans="1:5" x14ac:dyDescent="0.2">
@@ -1290,13 +1326,10 @@
         <v>10</v>
       </c>
       <c r="B51" t="s">
-        <v>82</v>
+        <v>57</v>
       </c>
       <c r="C51" t="s">
-        <v>83</v>
-      </c>
-      <c r="E51">
-        <v>502.50299999999999</v>
+        <v>59</v>
       </c>
     </row>
     <row r="52" spans="1:5" x14ac:dyDescent="0.2">
@@ -1304,10 +1337,13 @@
         <v>10</v>
       </c>
       <c r="B52" t="s">
-        <v>58</v>
+        <v>82</v>
       </c>
       <c r="C52" t="s">
-        <v>60</v>
+        <v>83</v>
+      </c>
+      <c r="E52">
+        <v>502.50299999999999</v>
       </c>
     </row>
     <row r="53" spans="1:5" x14ac:dyDescent="0.2">
@@ -1315,24 +1351,24 @@
         <v>10</v>
       </c>
       <c r="B53" t="s">
-        <v>70</v>
+        <v>58</v>
       </c>
       <c r="C53" t="s">
-        <v>71</v>
-      </c>
-      <c r="E53" t="s">
-        <v>69</v>
+        <v>60</v>
       </c>
     </row>
     <row r="54" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A54" t="s">
-        <v>61</v>
+        <v>10</v>
       </c>
       <c r="B54" t="s">
-        <v>62</v>
+        <v>70</v>
       </c>
       <c r="C54" t="s">
-        <v>63</v>
+        <v>71</v>
+      </c>
+      <c r="E54" t="s">
+        <v>69</v>
       </c>
     </row>
     <row r="55" spans="1:5" x14ac:dyDescent="0.2">
@@ -1340,10 +1376,10 @@
         <v>61</v>
       </c>
       <c r="B55" t="s">
-        <v>64</v>
+        <v>62</v>
       </c>
       <c r="C55" t="s">
-        <v>65</v>
+        <v>63</v>
       </c>
     </row>
     <row r="56" spans="1:5" x14ac:dyDescent="0.2">
@@ -1351,10 +1387,10 @@
         <v>61</v>
       </c>
       <c r="B56" t="s">
-        <v>102</v>
+        <v>64</v>
       </c>
       <c r="C56" t="s">
-        <v>103</v>
+        <v>65</v>
       </c>
     </row>
     <row r="57" spans="1:5" x14ac:dyDescent="0.2">
@@ -1362,21 +1398,21 @@
         <v>61</v>
       </c>
       <c r="B57" t="s">
-        <v>105</v>
+        <v>102</v>
       </c>
       <c r="C57" t="s">
-        <v>106</v>
+        <v>103</v>
       </c>
     </row>
     <row r="58" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A58" t="s">
-        <v>73</v>
+        <v>61</v>
       </c>
       <c r="B58" t="s">
-        <v>75</v>
+        <v>105</v>
       </c>
       <c r="C58" t="s">
-        <v>72</v>
+        <v>106</v>
       </c>
     </row>
     <row r="59" spans="1:5" x14ac:dyDescent="0.2">
@@ -1384,10 +1420,10 @@
         <v>73</v>
       </c>
       <c r="B59" t="s">
-        <v>88</v>
+        <v>75</v>
       </c>
       <c r="C59" t="s">
-        <v>89</v>
+        <v>72</v>
       </c>
     </row>
     <row r="60" spans="1:5" x14ac:dyDescent="0.2">
@@ -1395,10 +1431,10 @@
         <v>73</v>
       </c>
       <c r="B60" t="s">
-        <v>90</v>
+        <v>88</v>
       </c>
       <c r="C60" t="s">
-        <v>91</v>
+        <v>89</v>
       </c>
     </row>
     <row r="61" spans="1:5" x14ac:dyDescent="0.2">
@@ -1406,10 +1442,10 @@
         <v>73</v>
       </c>
       <c r="B61" t="s">
-        <v>92</v>
+        <v>90</v>
       </c>
       <c r="C61" t="s">
-        <v>93</v>
+        <v>91</v>
       </c>
     </row>
     <row r="62" spans="1:5" x14ac:dyDescent="0.2">
@@ -1417,10 +1453,10 @@
         <v>73</v>
       </c>
       <c r="B62" t="s">
-        <v>94</v>
+        <v>92</v>
       </c>
       <c r="C62" t="s">
-        <v>95</v>
+        <v>93</v>
       </c>
     </row>
     <row r="63" spans="1:5" x14ac:dyDescent="0.2">
@@ -1428,21 +1464,21 @@
         <v>73</v>
       </c>
       <c r="B63" t="s">
-        <v>112</v>
+        <v>94</v>
       </c>
       <c r="C63" t="s">
-        <v>113</v>
+        <v>95</v>
       </c>
     </row>
     <row r="64" spans="1:5" x14ac:dyDescent="0.2">
       <c r="A64" t="s">
-        <v>98</v>
+        <v>73</v>
       </c>
       <c r="B64" t="s">
-        <v>99</v>
+        <v>112</v>
       </c>
       <c r="C64" t="s">
-        <v>95</v>
+        <v>113</v>
       </c>
     </row>
     <row r="65" spans="1:3" x14ac:dyDescent="0.2">
@@ -1450,21 +1486,21 @@
         <v>98</v>
       </c>
       <c r="B65" t="s">
-        <v>100</v>
+        <v>99</v>
       </c>
       <c r="C65" t="s">
-        <v>101</v>
+        <v>95</v>
       </c>
     </row>
     <row r="66" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A66" t="s">
-        <v>107</v>
+        <v>98</v>
       </c>
       <c r="B66" t="s">
-        <v>110</v>
+        <v>100</v>
       </c>
       <c r="C66" t="s">
-        <v>109</v>
+        <v>101</v>
       </c>
     </row>
     <row r="67" spans="1:3" x14ac:dyDescent="0.2">
@@ -1472,25 +1508,91 @@
         <v>107</v>
       </c>
       <c r="B67" t="s">
-        <v>108</v>
+        <v>110</v>
       </c>
       <c r="C67" t="s">
-        <v>111</v>
+        <v>109</v>
       </c>
     </row>
     <row r="68" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A68" t="s">
-        <v>98</v>
+        <v>107</v>
       </c>
       <c r="B68" t="s">
-        <v>115</v>
+        <v>108</v>
       </c>
       <c r="C68" t="s">
-        <v>114</v>
+        <v>111</v>
       </c>
     </row>
     <row r="69" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A69" t="s">
+        <v>98</v>
+      </c>
+      <c r="B69" t="s">
+        <v>115</v>
+      </c>
+      <c r="C69" t="s">
+        <v>114</v>
+      </c>
+    </row>
+    <row r="70" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A70" t="s">
+        <v>116</v>
+      </c>
+      <c r="B70" t="s">
+        <v>117</v>
+      </c>
+      <c r="C70" t="s">
+        <v>118</v>
+      </c>
+    </row>
+    <row r="71" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A71" t="s">
+        <v>116</v>
+      </c>
+      <c r="B71" t="s">
+        <v>121</v>
+      </c>
+      <c r="C71" t="s">
+        <v>122</v>
+      </c>
+    </row>
+    <row r="72" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A72" t="s">
+        <v>116</v>
+      </c>
+      <c r="B72" t="s">
+        <v>119</v>
+      </c>
+      <c r="C72" t="s">
+        <v>120</v>
+      </c>
+    </row>
+    <row r="73" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A73" t="s">
+        <v>116</v>
+      </c>
+      <c r="B73" t="s">
+        <v>123</v>
+      </c>
+      <c r="C73" t="s">
+        <v>124</v>
+      </c>
+    </row>
+    <row r="74" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A74" t="s">
+        <v>116</v>
+      </c>
+      <c r="B74" t="s">
+        <v>126</v>
+      </c>
+      <c r="C74" t="s">
+        <v>127</v>
+      </c>
+    </row>
+    <row r="75" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A75" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
maj TP06 cours 7
</commit_message>
<xml_diff>
--- a/inventaire_exos.xlsx
+++ b/inventaire_exos.xlsx
@@ -401,9 +401,6 @@
     <t>FIC-011</t>
   </si>
   <si>
-    <t>Lecture d'un texte</t>
-  </si>
-  <si>
     <t>consignes_TP6</t>
   </si>
   <si>
@@ -411,6 +408,9 @@
   </si>
   <si>
     <t>Résultats de l'Embrunman</t>
+  </si>
+  <si>
+    <t>Lecture et analyses des caractères d'un texte</t>
   </si>
 </sst>
 </file>
@@ -727,8 +727,8 @@
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:F75"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A50" workbookViewId="0">
-      <selection activeCell="C74" sqref="C74"/>
+    <sheetView tabSelected="1" topLeftCell="A47" workbookViewId="0">
+      <selection activeCell="C73" sqref="C73"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -810,7 +810,7 @@
         <v>50</v>
       </c>
       <c r="B6" t="s">
-        <v>125</v>
+        <v>124</v>
       </c>
       <c r="C6" t="s">
         <v>51</v>
@@ -1577,7 +1577,7 @@
         <v>123</v>
       </c>
       <c r="C73" t="s">
-        <v>124</v>
+        <v>127</v>
       </c>
     </row>
     <row r="74" spans="1:3" x14ac:dyDescent="0.2">
@@ -1585,10 +1585,10 @@
         <v>116</v>
       </c>
       <c r="B74" t="s">
+        <v>125</v>
+      </c>
+      <c r="C74" t="s">
         <v>126</v>
-      </c>
-      <c r="C74" t="s">
-        <v>127</v>
       </c>
     </row>
     <row r="75" spans="1:3" x14ac:dyDescent="0.2">

</xml_diff>

<commit_message>
maj cours equa diff
</commit_message>
<xml_diff>
--- a/inventaire_exos.xlsx
+++ b/inventaire_exos.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="5340" yWindow="460" windowWidth="16860" windowHeight="12280" tabRatio="500"/>
+    <workbookView xWindow="-31240" yWindow="-160" windowWidth="16860" windowHeight="12280" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="exos" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="307" uniqueCount="176">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="316" uniqueCount="183">
   <si>
     <t>Domaine</t>
   </si>
@@ -555,6 +555,27 @@
   </si>
   <si>
     <t>INT-003</t>
+  </si>
+  <si>
+    <t>equadiffs</t>
+  </si>
+  <si>
+    <t>EQD-004</t>
+  </si>
+  <si>
+    <t>Equation différentielles d'ordre 1</t>
+  </si>
+  <si>
+    <t>EQD-005</t>
+  </si>
+  <si>
+    <t>Equation différentielles d'ordre 2</t>
+  </si>
+  <si>
+    <t>EQD-006</t>
+  </si>
+  <si>
+    <t>Cinétique chimique</t>
   </si>
 </sst>
 </file>
@@ -889,10 +910,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F97"/>
+  <dimension ref="A1:F100"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A75" workbookViewId="0">
-      <selection activeCell="C97" sqref="C97"/>
+    <sheetView tabSelected="1" topLeftCell="A79" workbookViewId="0">
+      <selection activeCell="C100" sqref="C100"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2018,8 +2039,41 @@
         <v>174</v>
       </c>
     </row>
-    <row r="97" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="97" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
+        <v>176</v>
+      </c>
+      <c r="B97" t="s">
+        <v>177</v>
+      </c>
+      <c r="C97" t="s">
+        <v>178</v>
+      </c>
+    </row>
+    <row r="98" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A98" t="s">
+        <v>176</v>
+      </c>
+      <c r="B98" t="s">
+        <v>179</v>
+      </c>
+      <c r="C98" t="s">
+        <v>180</v>
+      </c>
+    </row>
+    <row r="99" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A99" t="s">
+        <v>176</v>
+      </c>
+      <c r="B99" t="s">
+        <v>181</v>
+      </c>
+      <c r="C99" t="s">
+        <v>182</v>
+      </c>
+    </row>
+    <row r="100" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A100" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
maj pivot de Guass
</commit_message>
<xml_diff>
--- a/inventaire_exos.xlsx
+++ b/inventaire_exos.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="0" yWindow="460" windowWidth="16860" windowHeight="12280" tabRatio="500"/>
+    <workbookView xWindow="2820" yWindow="460" windowWidth="16860" windowHeight="12280" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="exos" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="337" uniqueCount="198">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="349" uniqueCount="206">
   <si>
     <t>Domaine</t>
   </si>
@@ -621,6 +621,30 @@
   </si>
   <si>
     <t>Modèle proie-prédateurs de Lotka-Volterra</t>
+  </si>
+  <si>
+    <t>systemes</t>
+  </si>
+  <si>
+    <t>SYS-003</t>
+  </si>
+  <si>
+    <t>Résolution de systèmes</t>
+  </si>
+  <si>
+    <t>SYS-004</t>
+  </si>
+  <si>
+    <t>Inversion de matrice</t>
+  </si>
+  <si>
+    <t>SYS-005</t>
+  </si>
+  <si>
+    <t>SYS-006</t>
+  </si>
+  <si>
+    <t>Régression linéaire par la méthode des moindres carrés</t>
   </si>
 </sst>
 </file>
@@ -955,10 +979,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F107"/>
+  <dimension ref="A1:F111"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A83" workbookViewId="0">
-      <selection activeCell="C103" sqref="C103"/>
+    <sheetView tabSelected="1" topLeftCell="A91" workbookViewId="0">
+      <selection activeCell="C111" sqref="C111"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2196,6 +2220,50 @@
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A107" t="s">
+        <v>198</v>
+      </c>
+      <c r="B107" t="s">
+        <v>199</v>
+      </c>
+      <c r="C107" t="s">
+        <v>200</v>
+      </c>
+    </row>
+    <row r="108" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A108" t="s">
+        <v>198</v>
+      </c>
+      <c r="B108" t="s">
+        <v>201</v>
+      </c>
+      <c r="C108" t="s">
+        <v>202</v>
+      </c>
+    </row>
+    <row r="109" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A109" t="s">
+        <v>198</v>
+      </c>
+      <c r="B109" t="s">
+        <v>203</v>
+      </c>
+      <c r="C109" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="110" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A110" t="s">
+        <v>198</v>
+      </c>
+      <c r="B110" t="s">
+        <v>204</v>
+      </c>
+      <c r="C110" t="s">
+        <v>205</v>
+      </c>
+    </row>
+    <row r="111" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A111" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
maj ipt emilien TP13 et cours 4-3
</commit_message>
<xml_diff>
--- a/inventaire_exos.xlsx
+++ b/inventaire_exos.xlsx
@@ -9,7 +9,7 @@
     </mc:Choice>
   </mc:AlternateContent>
   <bookViews>
-    <workbookView xWindow="2820" yWindow="460" windowWidth="16860" windowHeight="12280" tabRatio="500"/>
+    <workbookView xWindow="34420" yWindow="580" windowWidth="16860" windowHeight="12280" tabRatio="500"/>
   </bookViews>
   <sheets>
     <sheet name="exos" sheetId="1" r:id="rId1"/>
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="355" uniqueCount="210">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="364" uniqueCount="217">
   <si>
     <t>Domaine</t>
   </si>
@@ -657,6 +657,27 @@
   </si>
   <si>
     <t>Modèle de trajectoire d'un chien par rapport à son maître</t>
+  </si>
+  <si>
+    <t>sql</t>
+  </si>
+  <si>
+    <t>SQL-004</t>
+  </si>
+  <si>
+    <t>Base de données sur les acteurs</t>
+  </si>
+  <si>
+    <t>pont_de_wheastone</t>
+  </si>
+  <si>
+    <t>Application de physique : pont de wheastone</t>
+  </si>
+  <si>
+    <t>polynome</t>
+  </si>
+  <si>
+    <t>Interpolation</t>
   </si>
 </sst>
 </file>
@@ -991,10 +1012,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F113"/>
+  <dimension ref="A1:F116"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A94" workbookViewId="0">
-      <selection activeCell="C105" sqref="C105"/>
+    <sheetView tabSelected="1" topLeftCell="A97" workbookViewId="0">
+      <selection activeCell="C114" sqref="C114"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2296,8 +2317,41 @@
         <v>205</v>
       </c>
     </row>
-    <row r="113" spans="1:1" x14ac:dyDescent="0.2">
+    <row r="113" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A113" t="s">
+        <v>198</v>
+      </c>
+      <c r="B113" t="s">
+        <v>213</v>
+      </c>
+      <c r="C113" t="s">
+        <v>214</v>
+      </c>
+    </row>
+    <row r="114" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A114" t="s">
+        <v>198</v>
+      </c>
+      <c r="B114" t="s">
+        <v>215</v>
+      </c>
+      <c r="C114" t="s">
+        <v>216</v>
+      </c>
+    </row>
+    <row r="115" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A115" t="s">
+        <v>210</v>
+      </c>
+      <c r="B115" t="s">
+        <v>211</v>
+      </c>
+      <c r="C115" t="s">
+        <v>212</v>
+      </c>
+    </row>
+    <row r="116" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A116" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>

<commit_message>
maj emilien probleme fin d'annee
</commit_message>
<xml_diff>
--- a/inventaire_exos.xlsx
+++ b/inventaire_exos.xlsx
@@ -27,7 +27,7 @@
 </file>
 
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
-<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="400" uniqueCount="240">
+<sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="409" uniqueCount="247">
   <si>
     <t>Domaine</t>
   </si>
@@ -747,6 +747,27 @@
   </si>
   <si>
     <t>Mesure d'une position par un accéléromètre</t>
+  </si>
+  <si>
+    <t>STATIO-006</t>
+  </si>
+  <si>
+    <t>Méthodes numériques</t>
+  </si>
+  <si>
+    <t>FIC-013</t>
+  </si>
+  <si>
+    <t>Lecture d'un fichier donnant les décimales de pi</t>
+  </si>
+  <si>
+    <t>problemes</t>
+  </si>
+  <si>
+    <t>puissance vélo</t>
+  </si>
+  <si>
+    <t>Analyse de la puissance d'un cycliste à partir d'un relevé GPS</t>
   </si>
 </sst>
 </file>
@@ -1081,10 +1102,10 @@
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
 <worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
-  <dimension ref="A1:F128"/>
+  <dimension ref="A1:F131"/>
   <sheetViews>
-    <sheetView tabSelected="1" topLeftCell="A93" workbookViewId="0">
-      <selection activeCell="C106" sqref="C106"/>
+    <sheetView tabSelected="1" topLeftCell="A117" workbookViewId="0">
+      <selection activeCell="C131" sqref="C131"/>
     </sheetView>
   </sheetViews>
   <sheetFormatPr baseColWidth="10" defaultRowHeight="16" x14ac:dyDescent="0.2"/>
@@ -2212,13 +2233,13 @@
     </row>
     <row r="97" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A97" t="s">
-        <v>137</v>
+        <v>116</v>
       </c>
       <c r="B97" t="s">
-        <v>138</v>
+        <v>242</v>
       </c>
       <c r="C97" t="s">
-        <v>139</v>
+        <v>243</v>
       </c>
     </row>
     <row r="98" spans="1:3" x14ac:dyDescent="0.2">
@@ -2226,21 +2247,21 @@
         <v>137</v>
       </c>
       <c r="B98" t="s">
-        <v>140</v>
+        <v>138</v>
       </c>
       <c r="C98" t="s">
-        <v>141</v>
+        <v>139</v>
       </c>
     </row>
     <row r="99" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A99" t="s">
-        <v>169</v>
+        <v>137</v>
       </c>
       <c r="B99" t="s">
-        <v>171</v>
+        <v>140</v>
       </c>
       <c r="C99" t="s">
-        <v>170</v>
+        <v>141</v>
       </c>
     </row>
     <row r="100" spans="1:3" x14ac:dyDescent="0.2">
@@ -2248,10 +2269,10 @@
         <v>169</v>
       </c>
       <c r="B100" t="s">
-        <v>172</v>
+        <v>171</v>
       </c>
       <c r="C100" t="s">
-        <v>173</v>
+        <v>170</v>
       </c>
     </row>
     <row r="101" spans="1:3" x14ac:dyDescent="0.2">
@@ -2259,10 +2280,10 @@
         <v>169</v>
       </c>
       <c r="B101" t="s">
-        <v>175</v>
+        <v>172</v>
       </c>
       <c r="C101" t="s">
-        <v>174</v>
+        <v>173</v>
       </c>
     </row>
     <row r="102" spans="1:3" x14ac:dyDescent="0.2">
@@ -2270,10 +2291,10 @@
         <v>169</v>
       </c>
       <c r="B102" t="s">
-        <v>194</v>
+        <v>175</v>
       </c>
       <c r="C102" t="s">
-        <v>195</v>
+        <v>174</v>
       </c>
     </row>
     <row r="103" spans="1:3" x14ac:dyDescent="0.2">
@@ -2281,10 +2302,10 @@
         <v>169</v>
       </c>
       <c r="B103" t="s">
-        <v>238</v>
+        <v>194</v>
       </c>
       <c r="C103" t="s">
-        <v>239</v>
+        <v>195</v>
       </c>
     </row>
     <row r="104" spans="1:3" x14ac:dyDescent="0.2">
@@ -2292,21 +2313,21 @@
         <v>169</v>
       </c>
       <c r="B104" t="s">
-        <v>206</v>
+        <v>238</v>
       </c>
       <c r="C104" t="s">
-        <v>207</v>
+        <v>239</v>
       </c>
     </row>
     <row r="105" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A105" t="s">
-        <v>176</v>
+        <v>169</v>
       </c>
       <c r="B105" t="s">
-        <v>177</v>
+        <v>206</v>
       </c>
       <c r="C105" t="s">
-        <v>178</v>
+        <v>207</v>
       </c>
     </row>
     <row r="106" spans="1:3" x14ac:dyDescent="0.2">
@@ -2314,10 +2335,10 @@
         <v>176</v>
       </c>
       <c r="B106" t="s">
-        <v>179</v>
+        <v>177</v>
       </c>
       <c r="C106" t="s">
-        <v>180</v>
+        <v>178</v>
       </c>
     </row>
     <row r="107" spans="1:3" x14ac:dyDescent="0.2">
@@ -2325,10 +2346,10 @@
         <v>176</v>
       </c>
       <c r="B107" t="s">
-        <v>181</v>
+        <v>179</v>
       </c>
       <c r="C107" t="s">
-        <v>182</v>
+        <v>180</v>
       </c>
     </row>
     <row r="108" spans="1:3" x14ac:dyDescent="0.2">
@@ -2336,10 +2357,10 @@
         <v>176</v>
       </c>
       <c r="B108" t="s">
-        <v>183</v>
+        <v>181</v>
       </c>
       <c r="C108" t="s">
-        <v>184</v>
+        <v>182</v>
       </c>
     </row>
     <row r="109" spans="1:3" x14ac:dyDescent="0.2">
@@ -2347,10 +2368,10 @@
         <v>176</v>
       </c>
       <c r="B109" t="s">
-        <v>196</v>
+        <v>183</v>
       </c>
       <c r="C109" t="s">
-        <v>197</v>
+        <v>184</v>
       </c>
     </row>
     <row r="110" spans="1:3" x14ac:dyDescent="0.2">
@@ -2358,21 +2379,21 @@
         <v>176</v>
       </c>
       <c r="B110" t="s">
-        <v>208</v>
+        <v>196</v>
       </c>
       <c r="C110" t="s">
-        <v>209</v>
+        <v>197</v>
       </c>
     </row>
     <row r="111" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A111" t="s">
-        <v>185</v>
+        <v>176</v>
       </c>
       <c r="B111" t="s">
-        <v>186</v>
+        <v>208</v>
       </c>
       <c r="C111" t="s">
-        <v>191</v>
+        <v>209</v>
       </c>
     </row>
     <row r="112" spans="1:3" x14ac:dyDescent="0.2">
@@ -2380,10 +2401,10 @@
         <v>185</v>
       </c>
       <c r="B112" t="s">
-        <v>189</v>
+        <v>186</v>
       </c>
       <c r="C112" t="s">
-        <v>190</v>
+        <v>191</v>
       </c>
     </row>
     <row r="113" spans="1:3" x14ac:dyDescent="0.2">
@@ -2391,10 +2412,10 @@
         <v>185</v>
       </c>
       <c r="B113" t="s">
-        <v>188</v>
+        <v>189</v>
       </c>
       <c r="C113" t="s">
-        <v>187</v>
+        <v>190</v>
       </c>
     </row>
     <row r="114" spans="1:3" x14ac:dyDescent="0.2">
@@ -2402,10 +2423,10 @@
         <v>185</v>
       </c>
       <c r="B114" t="s">
-        <v>192</v>
+        <v>188</v>
       </c>
       <c r="C114" t="s">
-        <v>193</v>
+        <v>187</v>
       </c>
     </row>
     <row r="115" spans="1:3" x14ac:dyDescent="0.2">
@@ -2413,32 +2434,32 @@
         <v>185</v>
       </c>
       <c r="B115" t="s">
-        <v>219</v>
+        <v>192</v>
       </c>
       <c r="C115" t="s">
-        <v>220</v>
+        <v>193</v>
       </c>
     </row>
     <row r="116" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A116" t="s">
-        <v>198</v>
+        <v>185</v>
       </c>
       <c r="B116" t="s">
-        <v>199</v>
+        <v>219</v>
       </c>
       <c r="C116" t="s">
-        <v>200</v>
+        <v>220</v>
       </c>
     </row>
     <row r="117" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A117" t="s">
-        <v>198</v>
+        <v>185</v>
       </c>
       <c r="B117" t="s">
-        <v>201</v>
+        <v>240</v>
       </c>
       <c r="C117" t="s">
-        <v>202</v>
+        <v>241</v>
       </c>
     </row>
     <row r="118" spans="1:3" x14ac:dyDescent="0.2">
@@ -2446,10 +2467,10 @@
         <v>198</v>
       </c>
       <c r="B118" t="s">
-        <v>203</v>
+        <v>199</v>
       </c>
       <c r="C118" t="s">
-        <v>205</v>
+        <v>200</v>
       </c>
     </row>
     <row r="119" spans="1:3" x14ac:dyDescent="0.2">
@@ -2457,10 +2478,10 @@
         <v>198</v>
       </c>
       <c r="B119" t="s">
-        <v>204</v>
+        <v>201</v>
       </c>
       <c r="C119" t="s">
-        <v>205</v>
+        <v>202</v>
       </c>
     </row>
     <row r="120" spans="1:3" x14ac:dyDescent="0.2">
@@ -2468,10 +2489,10 @@
         <v>198</v>
       </c>
       <c r="B120" t="s">
-        <v>221</v>
+        <v>203</v>
       </c>
       <c r="C120" t="s">
-        <v>222</v>
+        <v>205</v>
       </c>
     </row>
     <row r="121" spans="1:3" x14ac:dyDescent="0.2">
@@ -2479,10 +2500,10 @@
         <v>198</v>
       </c>
       <c r="B121" t="s">
-        <v>213</v>
+        <v>204</v>
       </c>
       <c r="C121" t="s">
-        <v>214</v>
+        <v>205</v>
       </c>
     </row>
     <row r="122" spans="1:3" x14ac:dyDescent="0.2">
@@ -2490,10 +2511,10 @@
         <v>198</v>
       </c>
       <c r="B122" t="s">
-        <v>215</v>
+        <v>221</v>
       </c>
       <c r="C122" t="s">
-        <v>216</v>
+        <v>222</v>
       </c>
     </row>
     <row r="123" spans="1:3" x14ac:dyDescent="0.2">
@@ -2501,32 +2522,32 @@
         <v>198</v>
       </c>
       <c r="B123" t="s">
-        <v>217</v>
+        <v>213</v>
       </c>
       <c r="C123" t="s">
-        <v>218</v>
+        <v>214</v>
       </c>
     </row>
     <row r="124" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A124" t="s">
-        <v>210</v>
+        <v>198</v>
       </c>
       <c r="B124" t="s">
-        <v>211</v>
+        <v>215</v>
       </c>
       <c r="C124" t="s">
-        <v>212</v>
+        <v>216</v>
       </c>
     </row>
     <row r="125" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A125" t="s">
-        <v>210</v>
+        <v>198</v>
       </c>
       <c r="B125" t="s">
-        <v>224</v>
+        <v>217</v>
       </c>
       <c r="C125" t="s">
-        <v>225</v>
+        <v>218</v>
       </c>
     </row>
     <row r="126" spans="1:3" x14ac:dyDescent="0.2">
@@ -2534,10 +2555,10 @@
         <v>210</v>
       </c>
       <c r="B126" t="s">
-        <v>226</v>
+        <v>211</v>
       </c>
       <c r="C126" t="s">
-        <v>227</v>
+        <v>212</v>
       </c>
     </row>
     <row r="127" spans="1:3" x14ac:dyDescent="0.2">
@@ -2545,14 +2566,47 @@
         <v>210</v>
       </c>
       <c r="B127" t="s">
-        <v>228</v>
+        <v>224</v>
       </c>
       <c r="C127" t="s">
-        <v>229</v>
+        <v>225</v>
       </c>
     </row>
     <row r="128" spans="1:3" x14ac:dyDescent="0.2">
       <c r="A128" t="s">
+        <v>210</v>
+      </c>
+      <c r="B128" t="s">
+        <v>226</v>
+      </c>
+      <c r="C128" t="s">
+        <v>227</v>
+      </c>
+    </row>
+    <row r="129" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A129" t="s">
+        <v>210</v>
+      </c>
+      <c r="B129" t="s">
+        <v>228</v>
+      </c>
+      <c r="C129" t="s">
+        <v>229</v>
+      </c>
+    </row>
+    <row r="130" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A130" t="s">
+        <v>244</v>
+      </c>
+      <c r="B130" t="s">
+        <v>245</v>
+      </c>
+      <c r="C130" t="s">
+        <v>246</v>
+      </c>
+    </row>
+    <row r="131" spans="1:3" x14ac:dyDescent="0.2">
+      <c r="A131" t="s">
         <v>8</v>
       </c>
     </row>

</xml_diff>